<commit_message>
updated writing to excel code
</commit_message>
<xml_diff>
--- a/picks/bro_stats.xlsx
+++ b/picks/bro_stats.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Bro</t>
   </si>
   <si>
-    <t>Part 4 Score</t>
+    <t>Part2 Score</t>
+  </si>
+  <si>
+    <t>Part3 Score</t>
+  </si>
+  <si>
+    <t>Part4 Score</t>
   </si>
   <si>
     <t>Total</t>
@@ -360,15 +366,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,96 +384,150 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D2" t="n">
         <v>28</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
+        <v>18</v>
+      </c>
+      <c r="D3" t="n">
         <v>27</v>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>26</v>
+      </c>
+      <c r="C4" t="n">
+        <v>18</v>
+      </c>
+      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
+        <v>24</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="n">
+        <v>26</v>
+      </c>
+      <c r="E5" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" t="n">
+        <v>18</v>
+      </c>
+      <c r="D6" t="n">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="n">
-        <v>24</v>
-      </c>
-      <c r="C4" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="E6" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="n">
         <v>26</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" t="n">
+        <v>25</v>
+      </c>
+      <c r="E7" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="n">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="C8" t="n">
+        <v>18</v>
+      </c>
+      <c r="D8" t="n">
         <v>27</v>
       </c>
-      <c r="C6" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
-        <v>25</v>
-      </c>
-      <c r="C7" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="n">
-        <v>27</v>
-      </c>
-      <c r="C8" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n">
+        <v>26</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18</v>
+      </c>
+      <c r="D9" t="n">
         <v>30</v>
       </c>
-      <c r="C9" t="n">
-        <v>30</v>
+      <c r="E9" t="n">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>